<commit_message>
"Updated Sort012.java with Dutch National Flag comment, modified RotateArrayRight.java to rotate by 1 instead of 3, and updated FINAL450.xlsx."
</commit_message>
<xml_diff>
--- a/CodeHelp/FINAL450.xlsx
+++ b/CodeHelp/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DSA-2024\CodeHelp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E349800A-6AFC-4A2C-A902-7F3EFA43407A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6E77A-06BD-47DE-8A81-FEAAFC4B78CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1425,13 +1425,16 @@
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> yes</t>
-  </si>
-  <si>
     <t>S. no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -1509,18 +1512,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1563,8 +1560,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1883,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1913,7 +1910,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="11" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1943,7 +1940,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1957,7 +1954,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1971,7 +1968,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1985,7 +1982,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1999,7 +1996,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>3</v>
+        <v>466</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -2013,7 +2010,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>3</v>
+        <v>466</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -2027,7 +2024,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>3</v>
+        <v>466</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -2041,7 +2038,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>3</v>
+        <v>467</v>
       </c>
       <c r="D14">
         <v>9</v>

</xml_diff>

<commit_message>
add string manipulation algorithms and utility classes
</commit_message>
<xml_diff>
--- a/CodeHelp/FINAL450.xlsx
+++ b/CodeHelp/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DSA-2024\CodeHelp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6E77A-06BD-47DE-8A81-FEAAFC4B78CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BB34E6-AA66-49AB-8480-0077CE55DF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="2916" yWindow="624" windowWidth="17280" windowHeight="11076" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1512,12 +1512,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1533,7 +1539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1563,6 +1569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1570,6 +1577,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1880,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -2686,7 +2698,7 @@
       <c r="A68" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C68" s="4" t="s">

</xml_diff>